<commit_message>
update oracle sql sentences
</commit_message>
<xml_diff>
--- a/spring-social/queries/SQL Sentences in Oracle.xlsx
+++ b/spring-social/queries/SQL Sentences in Oracle.xlsx
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,8 +649,8 @@
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(1,'Inicio',1,'/',1,'home',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="O2" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+1,",",A2,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+2,",",A2,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+3,",",A2,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*4)+1,",",A2,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*5)+1,",",A2,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+1,",",A2,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (1,1,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (2,1,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (3,1,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (1,1,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (1,1,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (1,1,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+1,",",A2,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+2,",",A2,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+3,",",A2,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*4)+4,",",A2,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*5)+5,",",A2,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+6,",",A2,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (1,1,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (2,1,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (3,1,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (4,1,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (5,1,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (6,1,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -704,8 +704,8 @@
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(2,'Mi perfil',2,'/profile',1,'person',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O16" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+1,",",A3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+2,",",A3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+3,",",A3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*4)+1,",",A3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*5)+1,",",A3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+1,",",A3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (7,2,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (8,2,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (9,2,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (5,2,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (6,2,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (7,2,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" ref="O3:O15" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+1,",",A3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+2,",",A3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+3,",",A3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*4)+4,",",A3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*5)+5,",",A3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+6,",",A3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (7,2,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (8,2,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (9,2,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (8,2,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (10,2,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (12,2,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -760,7 +760,7 @@
       </c>
       <c r="O4" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (13,3,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (14,3,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (15,3,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (9,3,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (11,3,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (13,3,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (13,3,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (14,3,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (15,3,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (12,3,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (15,3,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (18,3,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -815,7 +815,7 @@
       </c>
       <c r="O5" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (19,4,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (20,4,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (21,4,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (13,4,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (16,4,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (19,4,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (19,4,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (20,4,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (21,4,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (16,4,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (20,4,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (24,4,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -870,7 +870,7 @@
       </c>
       <c r="O6" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (25,5,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (26,5,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (27,5,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (17,5,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (21,5,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (25,5,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (25,5,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (26,5,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (27,5,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (20,5,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (25,5,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (30,5,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -925,7 +925,7 @@
       </c>
       <c r="O7" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (31,6,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (32,6,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (33,6,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (21,6,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (26,6,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (31,6,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (31,6,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (32,6,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (33,6,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (24,6,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (30,6,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (36,6,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P7">
         <v>1</v>
@@ -980,7 +980,7 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (37,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (38,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (39,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (25,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (31,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (37,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (37,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (38,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (39,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (28,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (35,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (42,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P8">
         <v>1</v>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="O9" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (43,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (44,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (45,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (29,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (36,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (43,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (43,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (44,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (45,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (32,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (40,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (48,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P9">
         <v>1</v>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="O10" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (49,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (50,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (51,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (33,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (41,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (49,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (49,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (50,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (51,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (36,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (45,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (54,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (55,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (56,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (57,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (37,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (46,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (55,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (55,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (56,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (57,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (40,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (50,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (60,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P11">
         <v>1</v>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (61,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (62,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (63,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (41,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (51,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (61,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (61,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (62,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (63,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (44,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (55,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (66,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P12">
         <v>1</v>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="O13" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (67,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (68,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (69,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (45,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (56,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (67,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (67,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (68,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (69,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (48,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (60,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (72,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P13">
         <v>1</v>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (73,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (74,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (75,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (49,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (61,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (73,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (73,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (74,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (75,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (52,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (65,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (78,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P14">
         <v>1</v>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (79,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (80,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (81,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (53,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (66,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (79,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (79,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (80,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (81,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (56,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (70,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (84,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="P15">
         <v>1</v>

</xml_diff>

<commit_message>
add sequence code to models and update sql sentences
</commit_message>
<xml_diff>
--- a/spring-social/queries/SQL Sentences in Oracle.xlsx
+++ b/spring-social/queries/SQL Sentences in Oracle.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="67">
   <si>
     <t>rol_id</t>
   </si>
@@ -210,6 +210,24 @@
   <si>
     <t xml:space="preserve">ROL_FORM_ACTION </t>
   </si>
+  <si>
+    <t>SEQUENCY</t>
+  </si>
+  <si>
+    <t>form_sequence.nextval</t>
+  </si>
+  <si>
+    <t>FORM_ACTION_SEQUENCE</t>
+  </si>
+  <si>
+    <t>form_action_sequence.nextval</t>
+  </si>
+  <si>
+    <t>ROL_FORM_ACTION_SEQUENCE</t>
+  </si>
+  <si>
+    <t>ROL_FORM_ACTION_SEQUENCE.nextval</t>
+  </si>
 </sst>
 </file>
 
@@ -244,11 +262,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,868 +548,1011 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O15"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
-    <col min="14" max="14" width="60.28515625" customWidth="1"/>
-    <col min="15" max="15" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" customWidth="1"/>
+    <col min="15" max="15" width="60.28515625" customWidth="1"/>
+    <col min="16" max="16" width="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.140625" customWidth="1"/>
+    <col min="19" max="19" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>56</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>57</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" t="s">
         <v>58</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
+      <c r="H2">
+        <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>48</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="M2" t="str">
-        <f>+CONCATENATE(A1,",",B1,",",C1,",",D1,",",E1,",",F1,",",G1,",",H1,",",I1,",",J1,",",K1,",",L1)</f>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="str">
+        <f>+CONCATENATE(B1,",",C1,",",D1,",",E1,",",F1,",",G1,",",H1,",",I1,",",J1,",",K1,",",L1,",",M1)</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N2" t="str">
-        <f>+CONCATENATE("INSERT INTO form (",M2,") values(",A2,",'",B2,"',",C2,",'",D2,"',",E2,",'",F2,"',",G2,",",H2,",",I2,",",J2,",",K2,",'",L2,"');")</f>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(1,'Inicio',1,'/',1,'home',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O2" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+1,",",A2,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+2,",",A2,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+3,",",A2,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*4)+4,",",A2,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*5)+5,",",A2,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A2-1)*6)+6,",",A2,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (1,1,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (2,1,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (3,1,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (4,1,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (5,1,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (6,1,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
+        <f>+CONCATENATE("INSERT INTO form (",N2,") values(",A2,",'",C2,"',",D2,",'",E2,"',",F2,",'",G2,"',",H2,",",I2,",",J2,",",K2,",",L2,",'",M2,"');")</f>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',1,'/',1,'home',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P2" t="s">
+        <v>64</v>
       </c>
       <c r="Q2" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A2-1)*6)+1,",",((A2-1)*6)+1,",",P2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A2-1)*6)+2,",",((A2-1)*6)+2,",",P2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A2-1)*6)+3,",",((A2-1)*6)+3,",",P2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A2-1)*6)+4,",",((A2-1)*6)+4,",",P2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A2-1)*6)+5,",",((A2-1)*6)+5,",",P2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A2-1)*6)+6,",",((A2-1)*6)+6,",",P2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (1,1,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (2,2,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (3,3,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (4,4,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (5,5,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (6,6,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>+A2+1</f>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,1,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,1,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,1,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,1,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,1,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,1,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" t="str">
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+1,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+2,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+3,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+4,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+5,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+6,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,1,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,2,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,3,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,4,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,5,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,6,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <f>+B2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
+      <c r="H3">
+        <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
         <v>48</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="M3" t="str">
-        <f>+M2</f>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="str">
+        <f>+N2</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N15" si="0">+CONCATENATE("INSERT INTO form (",M3,") values(",A3,",'",B3,"',",C3,",'",D3,"',",E3,",'",F3,"',",G3,",",H3,",",I3,",",J3,",",K3,",'",L3,"');")</f>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(2,'Mi perfil',2,'/profile',1,'person',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O15" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+1,",",A3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+2,",",A3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+3,",",A3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*4)+4,",",A3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*5)+5,",",A3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",((A3-1)*6)+6,",",A3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (7,2,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (8,2,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (9,2,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (8,2,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (10,2,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (12,2,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
+        <f t="shared" ref="O3:O15" si="0">+CONCATENATE("INSERT INTO form (",N3,") values(",A3,",'",C3,"',",D3,",'",E3,"',",F3,",'",G3,"',",H3,",",I3,",",J3,",",K3,",",L3,",'",M3,"');")</f>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',2,'/profile',1,'person',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P3" t="s">
+        <v>64</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q15" si="2">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A3-1)*6)+1,",",((A3-1)*6)+1,",",P3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A3-1)*6)+2,",",((A3-1)*6)+2,",",P3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A3-1)*6)+3,",",((A3-1)*6)+3,",",P3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A3-1)*6)+4,",",((A3-1)*6)+4,",",P3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A3-1)*6)+5,",",((A3-1)*6)+5,",",P3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",((A3-1)*6)+6,",",((A3-1)*6)+6,",",P3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (7,7,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (8,8,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (9,9,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (10,10,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (11,11,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (12,12,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" ref="A4:A15" si="3">+A3+1</f>
+        <f t="shared" ref="Q3:Q15" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:T15" si="2">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+1,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+2,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+3,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+4,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+5,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+6,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,7,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,8,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,9,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,10,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,11,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,12,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B15" si="3">+B3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
+      <c r="H4">
+        <v>1</v>
       </c>
       <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
         <v>48</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="M4" t="str">
-        <f t="shared" ref="M4:M15" si="4">+M3</f>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N15" si="4">+N3</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(3,'Usuarios',2,'/user',1,'people',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O4" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (13,3,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (14,3,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (15,3,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (12,3,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (15,3,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (18,3,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Usuarios',2,'/user',1,'people',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P4" t="s">
+        <v>64</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (13,13,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (14,14,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (15,15,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (16,16,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (17,17,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (18,18,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,3,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,3,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,3,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,3,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,3,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,3,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>66</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,13,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,14,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,15,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,16,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,17,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,18,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>32</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>33</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
+      <c r="H5">
+        <v>1</v>
       </c>
       <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
         <v>48</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="M5" t="str">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="N5" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(4,'Roles',2,'/rol',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O5" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (19,4,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (20,4,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (21,4,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (16,4,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (20,4,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (24,4,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Roles',2,'/rol',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P5" t="s">
+        <v>64</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (19,19,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (20,20,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (21,21,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (22,22,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (23,23,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (24,24,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,4,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,4,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,4,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,4,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,4,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,4,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>66</v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,19,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,20,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,21,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,22,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,23,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,24,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>35</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>33</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
+      <c r="H6">
+        <v>1</v>
       </c>
       <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
         <v>48</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="M6" t="str">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="N6" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(5,'Acciones de roles',2,'/rolFormAction',0,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O6" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (25,5,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (26,5,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (27,5,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (20,5,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (25,5,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (30,5,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones de roles',2,'/rolFormAction',0,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P6" t="s">
+        <v>64</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (25,25,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (26,26,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (27,27,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (28,28,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (29,29,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (30,30,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,5,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,5,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,5,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,5,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,5,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,5,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>66</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,25,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,26,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,27,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,28,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,29,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,30,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>37</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>33</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
+      <c r="H7">
+        <v>1</v>
       </c>
       <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
         <v>48</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="M7" t="str">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(6,'Acciones por formulario',2,'/formAction',0,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O7" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (31,6,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (32,6,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (33,6,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (24,6,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (30,6,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (36,6,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones por formulario',2,'/formAction',0,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P7" t="s">
+        <v>64</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (31,31,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (32,32,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (33,33,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (34,34,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (35,35,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (36,36,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,31,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,32,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,33,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,34,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,35,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,36,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>40</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
+      <c r="H8">
+        <v>1</v>
       </c>
       <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
         <v>48</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="M8" t="str">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="N8" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(7,'Formularios',2,'/form',1,'chrome_reader_mode',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O8" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (37,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (38,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (39,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (28,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (35,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (42,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Formularios',2,'/form',1,'chrome_reader_mode',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P8" t="s">
+        <v>64</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (37,37,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (38,38,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (39,39,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (40,40,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (41,41,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (42,42,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>66</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,37,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,38,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,39,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,40,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,41,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,42,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>49</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>51</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
+      <c r="H9">
+        <v>1</v>
       </c>
       <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
         <v>48</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="M9" t="str">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(8,'Sistemas',2,'/system',1,'desktop_windows',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O9" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (43,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (44,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (45,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (32,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (40,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (48,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Sistemas',2,'/system',1,'desktop_windows',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P9" t="s">
+        <v>64</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (43,43,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (44,44,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (45,45,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (46,46,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (47,47,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (48,48,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>66</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,43,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,44,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,45,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,46,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,47,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,48,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>42</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
         <v>43</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
+      <c r="H10">
+        <v>1</v>
       </c>
       <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
         <v>48</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="M10" t="str">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N10" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(9,'Barriles',1,'/barril',1,'delete_outline',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O10" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (49,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (50,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (51,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (36,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (45,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (54,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',1,'/barril',1,'delete_outline',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P10" t="s">
+        <v>64</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (49,49,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (50,50,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (51,51,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (52,52,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (53,53,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (54,54,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,49,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,50,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,51,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,52,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,53,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,54,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
         <v>46</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
+      <c r="H11">
+        <v>1</v>
       </c>
       <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
         <v>48</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="M11" t="str">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="N11" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(10,'Tarimas',1,'/tarima',1,'dns',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
-      </c>
       <c r="O11" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (55,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (56,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (57,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (40,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (50,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (60,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',1,'/tarima',1,'dns',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+      </c>
+      <c r="P11" t="s">
+        <v>64</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (55,55,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (56,56,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (57,57,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (58,58,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (59,59,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (60,60,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11" t="s">
+        <v>66</v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,55,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,56,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,57,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,58,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,59,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,60,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>2</v>
       </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
       <c r="I12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" t="s">
         <v>48</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
         <v>52</v>
       </c>
-      <c r="M12" t="str">
+      <c r="N12" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N12" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(11,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
-      </c>
       <c r="O12" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (61,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (62,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (63,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (44,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (55,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (66,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
+      </c>
+      <c r="P12" t="s">
+        <v>64</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (61,61,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (62,62,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (63,63,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (64,64,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (65,65,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (66,66,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12" t="s">
+        <v>66</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,61,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,62,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,63,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,64,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,65,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,66,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>7</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>26</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
         <v>27</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>2</v>
       </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
       <c r="I13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" t="s">
         <v>48</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
         <v>53</v>
       </c>
-      <c r="M13" t="str">
+      <c r="N13" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(12,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
-      </c>
       <c r="O13" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (67,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (68,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (69,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (48,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (60,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (72,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
+      </c>
+      <c r="P13" t="s">
+        <v>64</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (67,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (68,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (69,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (70,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (71,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (72,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
+        <v>66</v>
+      </c>
+      <c r="T13" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>42</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>47</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>2</v>
       </c>
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
       <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
         <v>48</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
         <v>54</v>
       </c>
-      <c r="M14" t="str">
+      <c r="N14" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N14" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(13,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
-      </c>
       <c r="O14" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (73,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (74,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (75,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (52,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (65,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (78,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
+      </c>
+      <c r="P14" t="s">
+        <v>64</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (73,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (74,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (75,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (76,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (77,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (78,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>66</v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>46</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
       <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
         <v>48</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
         <v>55</v>
       </c>
-      <c r="M15" t="str">
+      <c r="N15" t="str">
         <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
-      <c r="N15" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(14,'Tarimas',9,'/tarima',1,'dns',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Pallet');</v>
-      </c>
       <c r="O15" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (79,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (80,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (81,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (56,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (70,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (84,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',9,'/tarima',1,'dns',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Pallet');</v>
+      </c>
+      <c r="P15" t="s">
+        <v>64</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (79,79,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (80,80,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (81,81,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (82,82,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (83,83,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (84,84,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15" t="s">
+        <v>66</v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,79,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,80,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,81,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,82,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,83,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,84,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="19" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <f>((B6-1)*6)+5</f>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L14">
+  <sortState ref="B2:M14">
+    <sortCondition ref="D2:D14"/>
     <sortCondition ref="C2:C14"/>
-    <sortCondition ref="B2:B14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add formGroup to sentences sql in script and excel file
</commit_message>
<xml_diff>
--- a/spring-social/queries/SQL Sentences in Oracle.xlsx
+++ b/spring-social/queries/SQL Sentences in Oracle.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="69">
   <si>
     <t>rol_id</t>
   </si>
@@ -130,9 +130,6 @@
     <t>supervised_user_circle</t>
   </si>
   <si>
-    <t>Acciones de roles</t>
-  </si>
-  <si>
     <t>/rolFormAction</t>
   </si>
   <si>
@@ -227,6 +224,15 @@
   </si>
   <si>
     <t>ROL_FORM_ACTION_SEQUENCE.nextval</t>
+  </si>
+  <si>
+    <t>Grupo de formularios</t>
+  </si>
+  <si>
+    <t>Acciones de rol</t>
+  </si>
+  <si>
+    <t>/formGroup</t>
   </si>
 </sst>
 </file>
@@ -548,15 +554,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -576,7 +583,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -615,30 +622,30 @@
         <v>20</v>
       </c>
       <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
         <v>56</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" t="s">
         <v>57</v>
       </c>
-      <c r="P1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>58</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" t="s">
         <v>59</v>
-      </c>
-      <c r="S1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -665,7 +672,7 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -682,7 +689,7 @@
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',1,'/',1,'home',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q2" t="str">
         <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P2,",",B2,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
@@ -692,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T2" t="str">
         <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+1,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+2,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+3,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+4,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+5,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S2,",",((B2-1)*6)+6,",",R2,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
@@ -701,7 +708,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <f>+B2+1</f>
@@ -729,7 +736,7 @@
         <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -742,33 +749,33 @@
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O15" si="0">+CONCATENATE("INSERT INTO form (",N3,") values(",A3,",'",C3,"',",D3,",'",E3,"',",F3,",'",G3,"',",H3,",",I3,",",J3,",",K3,",",L3,",'",M3,"');")</f>
+        <f t="shared" ref="O3:O16" si="0">+CONCATENATE("INSERT INTO form (",N3,") values(",A3,",'",C3,"',",D3,",'",E3,"',",F3,",'",G3,"',",H3,",",I3,",",J3,",",K3,",",L3,",'",M3,"');")</f>
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',2,'/profile',1,'person',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q15" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <f t="shared" ref="Q3:Q16" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
         <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T3" t="str">
-        <f t="shared" ref="T3:T15" si="2">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+1,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+2,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+3,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+4,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+5,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+6,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <f t="shared" ref="T3:T16" si="2">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+1,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+2,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+3,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+4,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+5,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+6,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,7,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,8,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,9,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,10,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,11,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,12,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B15" si="3">+B3+1</f>
+        <f t="shared" ref="B4:B16" si="3">+B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -793,7 +800,7 @@
         <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -802,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N15" si="4">+N3</f>
+        <f t="shared" ref="N4:N16" si="4">+N3</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O4" t="str">
@@ -810,7 +817,7 @@
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Usuarios',2,'/user',1,'people',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="1"/>
@@ -820,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="S4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T4" t="str">
         <f t="shared" si="2"/>
@@ -829,7 +836,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <f t="shared" si="3"/>
@@ -857,7 +864,7 @@
         <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -874,7 +881,7 @@
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Roles',2,'/rol',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="1"/>
@@ -884,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="S5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T5" t="str">
         <f t="shared" si="2"/>
@@ -893,20 +900,20 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -921,7 +928,7 @@
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -935,10 +942,10 @@
       </c>
       <c r="O6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones de roles',2,'/rolFormAction',0,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones de rol',2,'/rolFormAction',0,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="1"/>
@@ -948,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T6" t="str">
         <f t="shared" si="2"/>
@@ -957,20 +964,20 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -985,7 +992,7 @@
         <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1002,7 +1009,7 @@
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones por formulario',2,'/formAction',0,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="1"/>
@@ -1012,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="S7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T7" t="str">
         <f t="shared" si="2"/>
@@ -1021,26 +1028,26 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8">
-        <f t="shared" si="3"/>
+        <f>+B7+1</f>
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1049,7 +1056,7 @@
         <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1062,49 +1069,49 @@
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Formularios',2,'/form',1,'chrome_reader_mode',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <f t="shared" ref="O8" si="5">+CONCATENATE("INSERT INTO form (",N8,") values(",A8,",'",C8,"',",D8,",'",E8,"',",F8,",'",G8,"',",H8,",",I8,",",J8,",",K8,",",L8,",'",M8,"');")</f>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Grupo de formularios',2,'/formGroup',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q8" si="6">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
         <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R8">
         <v>1</v>
       </c>
       <c r="S8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="T8" si="7">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+1,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+2,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+3,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+4,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+5,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+6,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,37,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,38,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,39,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,40,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,41,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,42,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9">
-        <f t="shared" si="3"/>
+        <f>+B8+1</f>
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1113,7 +1120,7 @@
         <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1122,53 +1129,53 @@
         <v>0</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="4"/>
+        <f>+N7</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Sistemas',2,'/system',1,'desktop_windows',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Formularios',2,'/form',1,'chrome_reader_mode',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R9">
         <v>1</v>
       </c>
       <c r="S9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T9" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,43,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,44,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,45,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,46,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,47,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,48,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+1,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+2,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+3,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+4,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+5,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+6,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,37,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,38,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,39,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,40,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,41,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,42,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10">
-        <f t="shared" si="3"/>
+        <f>+B9+1</f>
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1177,7 +1184,7 @@
         <v>13</v>
       </c>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1191,48 +1198,48 @@
       </c>
       <c r="O10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',1,'/barril',1,'delete_outline',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Sistemas',2,'/system',1,'desktop_windows',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R10">
         <v>1</v>
       </c>
       <c r="S10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T10" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,49,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,50,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,51,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,52,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,53,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,54,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+1,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+2,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+3,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+4,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+5,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+6,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,43,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,44,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,45,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,46,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,47,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,48,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11">
-        <f t="shared" si="3"/>
+        <f>+B10+1</f>
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1241,7 +1248,7 @@
         <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1255,66 +1262,63 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',1,'/tarima',1,'dns',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',1,'/barril',1,'delete_outline',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R11">
         <v>1</v>
       </c>
       <c r="S11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T11" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,55,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,56,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,57,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,58,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,59,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,60,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+1,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+2,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+3,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+4,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+5,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+6,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,49,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,50,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,51,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,52,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,53,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,54,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12">
-        <f t="shared" si="3"/>
+        <f>+B11+1</f>
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" t="s">
         <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
         <v>0</v>
-      </c>
-      <c r="M12" t="s">
-        <v>52</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="4"/>
@@ -1322,48 +1326,48 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',1,'/tarima',1,'dns',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R12">
         <v>1</v>
       </c>
       <c r="S12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T12" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,61,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,62,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,63,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,64,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,65,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,66,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+1,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+2,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+3,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+4,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+5,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+6,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,55,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,56,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,57,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,58,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,59,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,60,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13">
-        <f t="shared" si="3"/>
+        <f>+B12+1</f>
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H13">
         <v>2</v>
@@ -1372,7 +1376,7 @@
         <v>13</v>
       </c>
       <c r="J13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1381,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="4"/>
@@ -1389,48 +1393,48 @@
       </c>
       <c r="O13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
       </c>
       <c r="P13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R13">
         <v>1</v>
       </c>
       <c r="S13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T13" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+1,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+2,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+3,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+4,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+5,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+6,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,61,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,62,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,63,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,64,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,65,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,66,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14">
-        <f t="shared" si="3"/>
+        <f>+B13+1</f>
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -1439,7 +1443,7 @@
         <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1448,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="4"/>
@@ -1456,42 +1460,42 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
       </c>
       <c r="P14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R14">
         <v>1</v>
       </c>
       <c r="S14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T14" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+1,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+2,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+3,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+4,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+5,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+6,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15">
-        <f t="shared" si="3"/>
+        <f>+B14+1</f>
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1506,7 +1510,7 @@
         <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -1515,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="4"/>
@@ -1523,28 +1527,95 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
+      </c>
+      <c r="P15" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q15" t="str">
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15" t="s">
+        <v>65</v>
+      </c>
+      <c r="T15" t="str">
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+1,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+2,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+3,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+4,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+5,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+6,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16">
+        <f>+B15+1</f>
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="0"/>
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',9,'/tarima',1,'dns',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Pallet');</v>
       </c>
-      <c r="P15" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q15" t="str">
-        <f t="shared" si="1"/>
+      <c r="P16" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q16" t="str">
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
         <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15" t="s">
-        <v>66</v>
-      </c>
-      <c r="T15" t="str">
-        <f t="shared" si="2"/>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16" t="s">
+        <v>65</v>
+      </c>
+      <c r="T16" t="str">
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+1,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+2,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+3,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+4,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+5,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+6,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,79,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,80,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,81,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,82,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,83,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,84,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
-    <row r="19" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q19">
+    <row r="20" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q20">
         <f>((B6-1)*6)+5</f>
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
add action to sql senteces and excel file
</commit_message>
<xml_diff>
--- a/spring-social/queries/SQL Sentences in Oracle.xlsx
+++ b/spring-social/queries/SQL Sentences in Oracle.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="71">
   <si>
     <t>rol_id</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>/formGroup</t>
+  </si>
+  <si>
+    <t>/action</t>
+  </si>
+  <si>
+    <t>Acciones</t>
   </si>
 </sst>
 </file>
@@ -554,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -749,14 +755,14 @@
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O16" si="0">+CONCATENATE("INSERT INTO form (",N3,") values(",A3,",'",C3,"',",D3,",'",E3,"',",F3,",'",G3,"',",H3,",",I3,",",J3,",",K3,",",L3,",'",M3,"');")</f>
+        <f t="shared" ref="O3:O17" si="0">+CONCATENATE("INSERT INTO form (",N3,") values(",A3,",'",C3,"',",D3,",'",E3,"',",F3,",'",G3,"',",H3,",",I3,",",J3,",",K3,",",L3,",'",M3,"');")</f>
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',2,'/profile',1,'person',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P3" t="s">
         <v>63</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q16" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <f t="shared" ref="Q3:Q8" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
         <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R3">
@@ -766,7 +772,7 @@
         <v>65</v>
       </c>
       <c r="T3" t="str">
-        <f t="shared" ref="T3:T16" si="2">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+1,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+2,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+3,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+4,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+5,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+6,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <f t="shared" ref="T3:T8" si="2">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+1,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+2,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+3,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+4,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+5,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S3,",",((B3-1)*6)+6,",",R3,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,7,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,8,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,9,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,10,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,11,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,12,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
@@ -775,7 +781,7 @@
         <v>61</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B16" si="3">+B3+1</f>
+        <f t="shared" ref="B4:B6" si="3">+B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -809,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N16" si="4">+N3</f>
+        <f t="shared" ref="N4:N17" si="4">+N3</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O4" t="str">
@@ -967,20 +973,20 @@
         <v>61</v>
       </c>
       <c r="B7">
-        <f t="shared" si="3"/>
+        <f>+B6+1</f>
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
         <v>33</v>
@@ -1005,8 +1011,8 @@
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones por formulario',2,'/formAction',0,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <f t="shared" ref="O7" si="5">+CONCATENATE("INSERT INTO form (",N7,") values(",A7,",'",C7,"',",D7,",'",E7,"',",F7,",'",G7,"',",H7,",",I7,",",J7,",",K7,",",L7,",'",M7,"');")</f>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones',2,'/action',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P7" t="s">
         <v>63</v>
@@ -1035,13 +1041,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1065,19 +1071,19 @@
         <v>0</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="4"/>
+        <f>+N6</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" ref="O8" si="5">+CONCATENATE("INSERT INTO form (",N8,") values(",A8,",'",C8,"',",D8,",'",E8,"',",F8,",'",G8,"',",H8,",",I8,",",J8,",",K8,",",L8,",'",M8,"');")</f>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Grupo de formularios',2,'/formGroup',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones por formulario',2,'/formAction',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P8" t="s">
         <v>63</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" ref="Q8" si="6">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B8,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -1086,8 +1092,8 @@
         <v>65</v>
       </c>
       <c r="T8" t="str">
-        <f t="shared" ref="T8" si="7">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+1,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+2,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+3,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+4,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+5,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B8-1)*6)+6,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,37,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,38,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,39,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,40,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,41,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,42,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+1,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+2,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+3,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+4,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+5,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+6,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,31,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,32,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,33,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,34,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,35,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,36,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1099,19 +1105,19 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1129,12 +1135,12 @@
         <v>0</v>
       </c>
       <c r="N9" t="str">
-        <f>+N7</f>
+        <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Formularios',2,'/form',1,'chrome_reader_mode',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <f t="shared" ref="O9" si="6">+CONCATENATE("INSERT INTO form (",N9,") values(",A9,",'",C9,"',",D9,",'",E9,"',",F9,",'",G9,"',",H9,",",I9,",",J9,",",K9,",",L9,",'",M9,"');")</f>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Grupo de formularios',2,'/formGroup',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P9" t="s">
         <v>63</v>
@@ -1163,19 +1169,19 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1193,19 +1199,19 @@
         <v>0</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="4"/>
+        <f>+N8</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Sistemas',2,'/system',1,'desktop_windows',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Formularios',2,'/form',1,'chrome_reader_mode',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P10" t="s">
         <v>63</v>
       </c>
       <c r="Q10" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B9,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -1214,8 +1220,8 @@
         <v>65</v>
       </c>
       <c r="T10" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+1,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+2,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+3,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+4,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+5,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B9-1)*6)+6,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,43,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,44,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,45,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,46,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,47,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,48,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+1,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+2,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+3,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+4,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+5,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+6,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,37,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,38,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,39,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,40,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,41,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,42,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1227,19 +1233,19 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1262,14 +1268,14 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',1,'/barril',1,'delete_outline',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Sistemas',2,'/system',1,'desktop_windows',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P11" t="s">
         <v>63</v>
       </c>
       <c r="Q11" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B10,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R11">
         <v>1</v>
@@ -1278,8 +1284,8 @@
         <v>65</v>
       </c>
       <c r="T11" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+1,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+2,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+3,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+4,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+5,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B10-1)*6)+6,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,49,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,50,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,51,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,52,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,53,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,54,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+1,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+2,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+3,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+4,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+5,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+6,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,43,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,44,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,45,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,46,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,47,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,48,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1291,19 +1297,19 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1326,14 +1332,14 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',1,'/tarima',1,'dns',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',1,'/barril',1,'delete_outline',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P12" t="s">
         <v>63</v>
       </c>
       <c r="Q12" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B11,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R12">
         <v>1</v>
@@ -1342,8 +1348,8 @@
         <v>65</v>
       </c>
       <c r="T12" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+1,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+2,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+3,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+4,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+5,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B11-1)*6)+6,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,55,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,56,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,57,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,58,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,59,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,60,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+1,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+2,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+3,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+4,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+5,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+6,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,49,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,50,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,51,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,52,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,53,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,54,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1355,22 +1361,22 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
@@ -1383,9 +1389,6 @@
       </c>
       <c r="L13">
         <v>0</v>
-      </c>
-      <c r="M13" t="s">
-        <v>51</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="4"/>
@@ -1393,14 +1396,14 @@
       </c>
       <c r="O13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',1,'/tarima',1,'dns',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P13" t="s">
         <v>63</v>
       </c>
       <c r="Q13" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B12,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R13">
         <v>1</v>
@@ -1409,8 +1412,8 @@
         <v>65</v>
       </c>
       <c r="T13" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+1,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+2,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+3,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+4,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+5,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B12-1)*6)+6,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,61,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,62,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,63,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,64,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,65,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,66,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+1,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+2,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+3,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+4,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+5,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+6,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,55,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,56,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,57,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,58,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,59,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,60,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1422,19 +1425,19 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -1452,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="4"/>
@@ -1460,14 +1463,14 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
       </c>
       <c r="P14" t="s">
         <v>63</v>
       </c>
       <c r="Q14" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B13,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R14">
         <v>1</v>
@@ -1476,8 +1479,8 @@
         <v>65</v>
       </c>
       <c r="T14" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+1,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+2,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+3,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+4,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+5,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B13-1)*6)+6,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+1,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+2,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+3,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+4,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+5,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+6,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,61,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,62,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,63,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,64,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,65,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,66,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1489,19 +1492,19 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -1519,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="4"/>
@@ -1527,14 +1530,14 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
       </c>
       <c r="P15" t="s">
         <v>63</v>
       </c>
       <c r="Q15" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B14,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R15">
         <v>1</v>
@@ -1543,8 +1546,8 @@
         <v>65</v>
       </c>
       <c r="T15" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+1,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+2,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+3,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+4,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+5,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B14-1)*6)+6,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+1,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+2,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+3,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+4,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+5,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+6,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1556,19 +1559,19 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -1586,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="4"/>
@@ -1594,14 +1597,14 @@
       </c>
       <c r="O16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',9,'/tarima',1,'dns',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Pallet');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
       </c>
       <c r="P16" t="s">
         <v>63</v>
       </c>
       <c r="Q16" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B15,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -1610,12 +1613,79 @@
         <v>65</v>
       </c>
       <c r="T16" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+1,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+2,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+3,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+4,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+5,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B15-1)*6)+6,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+1,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+2,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+3,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+4,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+5,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+6,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17">
+        <f>+B16+1</f>
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>54</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',9,'/tarima',1,'dns',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Pallet');</v>
+      </c>
+      <c r="P17" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q17" t="str">
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17" t="s">
+        <v>65</v>
+      </c>
+      <c r="T17" t="str">
+        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+1,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+2,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+3,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+4,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+5,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+6,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,79,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,80,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,81,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,82,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,83,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,84,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
-    <row r="20" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q21">
         <f>((B6-1)*6)+5</f>
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
add method to sql queries
</commit_message>
<xml_diff>
--- a/spring-social/queries/SQL Sentences in Oracle.xlsx
+++ b/spring-social/queries/SQL Sentences in Oracle.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="73">
   <si>
     <t>rol_id</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>Acciones</t>
+  </si>
+  <si>
+    <t>Metodos</t>
+  </si>
+  <si>
+    <t>/method</t>
   </si>
 </sst>
 </file>
@@ -254,12 +260,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -274,12 +298,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,22 +658,22 @@
       <c r="N1" t="s">
         <v>55</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>56</v>
       </c>
       <c r="P1" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>57</v>
       </c>
       <c r="R1" t="s">
         <v>58</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="6" t="s">
         <v>59</v>
       </c>
     </row>
@@ -755,14 +783,14 @@
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O17" si="0">+CONCATENATE("INSERT INTO form (",N3,") values(",A3,",'",C3,"',",D3,",'",E3,"',",F3,",'",G3,"',",H3,",",I3,",",J3,",",K3,",",L3,",'",M3,"');")</f>
+        <f t="shared" ref="O3:O18" si="0">+CONCATENATE("INSERT INTO form (",N3,") values(",A3,",'",C3,"',",D3,",'",E3,"',",F3,",'",G3,"',",H3,",",I3,",",J3,",",K3,",",L3,",'",M3,"');")</f>
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',2,'/profile',1,'person',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P3" t="s">
         <v>63</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q8" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
+        <f t="shared" ref="Q3:Q18" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P3,",",B3,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
         <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,2,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R3">
@@ -781,7 +809,7 @@
         <v>61</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B6" si="3">+B3+1</f>
+        <f t="shared" ref="B4:B18" si="3">+B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -815,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N17" si="4">+N3</f>
+        <f t="shared" ref="N4:N18" si="4">+N3</f>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O4" t="str">
@@ -836,7 +864,7 @@
         <v>65</v>
       </c>
       <c r="T4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="T4:T18" si="5">CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S4,",",((B4-1)*6)+1,",",R4,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S4,",",((B4-1)*6)+2,",",R4,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S4,",",((B4-1)*6)+3,",",R4,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S4,",",((B4-1)*6)+4,",",R4,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S4,",",((B4-1)*6)+5,",",R4,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S4,",",((B4-1)*6)+6,",",R4,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,13,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,14,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,15,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,16,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,17,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,18,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
@@ -900,7 +928,7 @@
         <v>65</v>
       </c>
       <c r="T5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,19,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,20,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,21,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,22,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,23,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,24,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
@@ -964,7 +992,7 @@
         <v>65</v>
       </c>
       <c r="T6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,25,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,26,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,27,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,28,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,29,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,30,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
@@ -973,7 +1001,7 @@
         <v>61</v>
       </c>
       <c r="B7">
-        <f>+B6+1</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="C7" t="s">
@@ -1011,7 +1039,7 @@
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" ref="O7" si="5">+CONCATENATE("INSERT INTO form (",N7,") values(",A7,",'",C7,"',",D7,",'",E7,"',",F7,",'",G7,"',",H7,",",I7,",",J7,",",K7,",",L7,",'",M7,"');")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones',2,'/action',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P7" t="s">
@@ -1028,7 +1056,7 @@
         <v>65</v>
       </c>
       <c r="T7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,31,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,32,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,33,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,34,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,35,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,36,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
@@ -1037,17 +1065,17 @@
         <v>61</v>
       </c>
       <c r="B8">
-        <f>+B7+1</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1071,19 +1099,19 @@
         <v>0</v>
       </c>
       <c r="N8" t="str">
-        <f>+N6</f>
+        <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones por formulario',2,'/formAction',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Metodos',2,'/method',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P8" t="s">
         <v>63</v>
       </c>
       <c r="Q8" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P8,",",B7,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,6,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -1092,8 +1120,8 @@
         <v>65</v>
       </c>
       <c r="T8" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+1,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+2,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+3,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+4,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+5,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S8,",",((B7-1)*6)+6,",",R8,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,31,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,32,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,33,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,34,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,35,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,36,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,37,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,38,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,39,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,40,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,41,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,42,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1101,17 +1129,17 @@
         <v>61</v>
       </c>
       <c r="B9">
-        <f>+B8+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1139,15 +1167,15 @@
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" ref="O9" si="6">+CONCATENATE("INSERT INTO form (",N9,") values(",A9,",'",C9,"',",D9,",'",E9,"',",F9,",'",G9,"',",H9,",",I9,",",J9,",",K9,",",L9,",'",M9,"');")</f>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Grupo de formularios',2,'/formGroup',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Acciones por formulario',2,'/formAction',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P9" t="s">
         <v>63</v>
       </c>
       <c r="Q9" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P9,",",B8,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R9">
         <v>1</v>
@@ -1156,8 +1184,8 @@
         <v>65</v>
       </c>
       <c r="T9" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+1,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+2,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+3,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+4,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+5,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S9,",",((B8-1)*6)+6,",",R9,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,37,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,38,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,39,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,40,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,41,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,42,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,43,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,44,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,45,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,46,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,47,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,48,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1165,23 +1193,23 @@
         <v>61</v>
       </c>
       <c r="B10">
-        <f>+B9+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1199,19 +1227,19 @@
         <v>0</v>
       </c>
       <c r="N10" t="str">
-        <f>+N8</f>
+        <f t="shared" si="4"/>
         <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Formularios',2,'/form',1,'chrome_reader_mode',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Grupo de formularios',2,'/formGroup',1,'supervised_user_circle',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P10" t="s">
         <v>63</v>
       </c>
       <c r="Q10" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P10,",",B8,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,7,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -1220,8 +1248,8 @@
         <v>65</v>
       </c>
       <c r="T10" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+1,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+2,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+3,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+4,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+5,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S10,",",((B8-1)*6)+6,",",R10,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,37,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,38,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,39,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,40,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,41,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,42,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,49,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,50,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,51,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,52,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,53,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,54,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1229,23 +1257,23 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <f>+B10+1</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1268,14 +1296,14 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Sistemas',2,'/system',1,'desktop_windows',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Formularios',2,'/form',1,'chrome_reader_mode',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P11" t="s">
         <v>63</v>
       </c>
       <c r="Q11" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P11,",",B9,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,8,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R11">
         <v>1</v>
@@ -1284,8 +1312,8 @@
         <v>65</v>
       </c>
       <c r="T11" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+1,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+2,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+3,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+4,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+5,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S11,",",((B9-1)*6)+6,",",R11,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,43,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,44,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,45,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,46,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,47,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,48,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,55,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,56,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,57,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,58,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,59,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,60,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1293,23 +1321,23 @@
         <v>61</v>
       </c>
       <c r="B12">
-        <f>+B11+1</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1332,14 +1360,14 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',1,'/barril',1,'delete_outline',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Sistemas',2,'/system',1,'desktop_windows',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P12" t="s">
         <v>63</v>
       </c>
       <c r="Q12" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P12,",",B10,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,9,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R12">
         <v>1</v>
@@ -1348,8 +1376,8 @@
         <v>65</v>
       </c>
       <c r="T12" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+1,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+2,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+3,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+4,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+5,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S12,",",((B10-1)*6)+6,",",R12,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,49,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,50,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,51,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,52,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,53,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,54,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,61,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,62,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,63,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,64,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,65,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,66,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1357,23 +1385,23 @@
         <v>61</v>
       </c>
       <c r="B13">
-        <f>+B12+1</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1396,14 +1424,14 @@
       </c>
       <c r="O13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',1,'/tarima',1,'dns',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',1,'/barril',1,'delete_outline',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P13" t="s">
         <v>63</v>
       </c>
       <c r="Q13" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P13,",",B11,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,10,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R13">
         <v>1</v>
@@ -1412,8 +1440,8 @@
         <v>65</v>
       </c>
       <c r="T13" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+1,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+2,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+3,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+4,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+5,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S13,",",((B11-1)*6)+6,",",R13,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,55,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,56,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,57,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,58,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,59,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,60,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1421,26 +1449,26 @@
         <v>61</v>
       </c>
       <c r="B14">
-        <f>+B13+1</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" t="s">
         <v>13</v>
@@ -1453,9 +1481,6 @@
       </c>
       <c r="L14">
         <v>0</v>
-      </c>
-      <c r="M14" t="s">
-        <v>51</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="4"/>
@@ -1463,14 +1488,14 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',1,'/tarima',1,'dns',1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'');</v>
       </c>
       <c r="P14" t="s">
         <v>63</v>
       </c>
       <c r="Q14" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P14,",",B12,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,11,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R14">
         <v>1</v>
@@ -1479,8 +1504,8 @@
         <v>65</v>
       </c>
       <c r="T14" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+1,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+2,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+3,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+4,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+5,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S14,",",((B12-1)*6)+6,",",R14,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,61,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,62,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,63,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,64,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,65,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,66,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1488,23 +1513,23 @@
         <v>61</v>
       </c>
       <c r="B15">
-        <f>+B14+1</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -1522,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="4"/>
@@ -1530,14 +1555,14 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Inicio',6,'/',1,'home',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Home');</v>
       </c>
       <c r="P15" t="s">
         <v>63</v>
       </c>
       <c r="Q15" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P15,",",B13,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,12,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R15">
         <v>1</v>
@@ -1546,8 +1571,8 @@
         <v>65</v>
       </c>
       <c r="T15" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+1,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+2,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+3,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+4,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+5,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S15,",",((B13-1)*6)+6,",",R15,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,67,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,68,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,69,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,70,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,71,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,72,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,79,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,80,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,81,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,82,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,83,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,84,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1555,23 +1580,23 @@
         <v>61</v>
       </c>
       <c r="B16">
-        <f>+B15+1</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -1589,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="4"/>
@@ -1597,14 +1622,14 @@
       </c>
       <c r="O16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Mi perfil',7,'/profile',1,'person',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Profile');</v>
       </c>
       <c r="P16" t="s">
         <v>63</v>
       </c>
       <c r="Q16" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P16,",",B14,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,13,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,15,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -1613,8 +1638,8 @@
         <v>65</v>
       </c>
       <c r="T16" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+1,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+2,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+3,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+4,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+5,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S16,",",((B14-1)*6)+6,",",R16,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,73,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,74,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,75,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,76,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,77,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,78,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,85,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,86,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,87,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,88,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,89,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,90,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -1622,23 +1647,23 @@
         <v>61</v>
       </c>
       <c r="B17">
-        <f>+B16+1</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -1656,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="4"/>
@@ -1664,14 +1689,14 @@
       </c>
       <c r="O17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',9,'/tarima',1,'dns',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Pallet');</v>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Barriles',8,'/barril',1,'battery-full',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Barrel');</v>
       </c>
       <c r="P17" t="s">
         <v>63</v>
       </c>
       <c r="Q17" t="str">
-        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);","insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",P17,",",B15,",6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);")</f>
-        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,14,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,16,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
       <c r="R17">
         <v>1</v>
@@ -1680,12 +1705,79 @@
         <v>65</v>
       </c>
       <c r="T17" t="str">
-        <f>CONCATENATE("INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+1,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );","INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+2,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+3,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+4,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+5,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );", "INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (",S17,",",((B15-1)*6)+6,",",R17,",TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );")</f>
-        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,79,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,80,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,81,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,82,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,83,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,84,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q21">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,91,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,92,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,93,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,94,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,95,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,96,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>54</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="4"/>
+        <v>id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO form (id,name,form_group_id,path,show_in_menu,icon,system_id,created_at,updated_at,created_by,updated_by,mobile_screen) values(form_sequence.nextval,'Tarimas',9,'/tarima',1,'dns',2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),null,0,0,'Pallet');</v>
+      </c>
+      <c r="P18" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,2,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,3,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,4,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,5,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (form_action_sequence.nextval,17,6,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18" t="s">
+        <v>65</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,97,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,98,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,99,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,100,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,101,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );INSERT INTO ROL_FORM_ACTION (id,form_action_id,rol_id, created_at) values (ROL_FORM_ACTION_SEQUENCE.nextval,102,1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss') );</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q22">
         <f>((B6-1)*6)+5</f>
         <v>29</v>
       </c>

</xml_diff>